<commit_message>
New version. Also trying of analysis the distribution
</commit_message>
<xml_diff>
--- a/resault_table.xlsx
+++ b/resault_table.xlsx
@@ -1,28 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="765" yWindow="270" windowWidth="27390" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>f(n)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -34,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -42,25 +65,154 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +250,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -170,7 +322,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -343,36 +495,654 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:CX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:102" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1">
+        <v>12</v>
+      </c>
+      <c r="O2" s="1">
+        <v>13</v>
+      </c>
+      <c r="P2" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>15</v>
+      </c>
+      <c r="R2" s="1">
+        <v>16</v>
+      </c>
+      <c r="S2" s="1">
+        <v>17</v>
+      </c>
+      <c r="T2" s="1">
+        <v>18</v>
+      </c>
+      <c r="U2" s="1">
+        <v>19</v>
+      </c>
+      <c r="V2" s="1">
+        <v>20</v>
+      </c>
+      <c r="W2" s="1">
+        <v>21</v>
+      </c>
+      <c r="X2" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>39</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>41</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>42</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>43</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>44</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>45</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>46</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>47</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>48</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>49</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>50</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>51</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>52</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>53</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>54</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>55</v>
+      </c>
+      <c r="BF2" s="1">
+        <v>56</v>
+      </c>
+      <c r="BG2" s="1">
+        <v>57</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>58</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>59</v>
+      </c>
+      <c r="BJ2" s="1">
+        <v>60</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>61</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>62</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>63</v>
+      </c>
+      <c r="BN2" s="1">
+        <v>64</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>65</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>66</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>67</v>
+      </c>
+      <c r="BR2" s="1">
+        <v>68</v>
+      </c>
+      <c r="BS2" s="1">
+        <v>69</v>
+      </c>
+      <c r="BT2" s="1">
+        <v>70</v>
+      </c>
+      <c r="BU2" s="1">
+        <v>71</v>
+      </c>
+      <c r="BV2" s="1">
+        <v>72</v>
+      </c>
+      <c r="BW2" s="1">
+        <v>73</v>
+      </c>
+      <c r="BX2" s="1">
+        <v>74</v>
+      </c>
+      <c r="BY2" s="1">
+        <v>75</v>
+      </c>
+      <c r="BZ2" s="1">
+        <v>76</v>
+      </c>
+      <c r="CA2" s="1">
+        <v>77</v>
+      </c>
+      <c r="CB2" s="1">
+        <v>78</v>
+      </c>
+      <c r="CC2" s="1">
+        <v>79</v>
+      </c>
+      <c r="CD2" s="1">
+        <v>80</v>
+      </c>
+      <c r="CE2" s="1">
+        <v>81</v>
+      </c>
+      <c r="CF2" s="1">
+        <v>82</v>
+      </c>
+      <c r="CG2" s="1">
+        <v>83</v>
+      </c>
+      <c r="CH2" s="1">
+        <v>84</v>
+      </c>
+      <c r="CI2" s="1">
+        <v>85</v>
+      </c>
+      <c r="CJ2" s="1">
+        <v>86</v>
+      </c>
+      <c r="CK2" s="1">
+        <v>87</v>
+      </c>
+      <c r="CL2" s="1">
+        <v>88</v>
+      </c>
+      <c r="CM2" s="1">
+        <v>89</v>
+      </c>
+      <c r="CN2" s="1">
+        <v>90</v>
+      </c>
+      <c r="CO2" s="1">
+        <v>91</v>
+      </c>
+      <c r="CP2" s="1">
+        <v>92</v>
+      </c>
+      <c r="CQ2" s="1">
+        <v>93</v>
+      </c>
+      <c r="CR2" s="1">
+        <v>94</v>
+      </c>
+      <c r="CS2" s="1">
+        <v>95</v>
+      </c>
+      <c r="CT2" s="1">
+        <v>96</v>
+      </c>
+      <c r="CU2" s="1">
+        <v>97</v>
+      </c>
+      <c r="CV2" s="1">
+        <v>98</v>
+      </c>
+      <c r="CW2" s="1">
+        <v>99</v>
+      </c>
+      <c r="CX2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.00016593933105E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>9.9921226501464792E-3</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>9.9968910217285104E-3</v>
+      </c>
+      <c r="H3" s="3">
+        <v>3.0012130737304601E-2</v>
+      </c>
+      <c r="I3" s="3">
+        <v>3.0004978179931599E-2</v>
+      </c>
+      <c r="J3" s="3">
+        <v>3.0012130737304601E-2</v>
+      </c>
+      <c r="K3" s="3">
+        <v>4.00280952453613E-2</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1.99723243713378E-2</v>
+      </c>
+      <c r="M3" s="3">
+        <v>5.0034523010253899E-2</v>
+      </c>
+      <c r="N3" s="3">
+        <v>4.0011405944824198E-2</v>
+      </c>
+      <c r="O3" s="3">
+        <v>7.9970359802246094E-2</v>
+      </c>
+      <c r="P3" s="3">
+        <v>2.9981136322021401E-2</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>7.0056915283203097E-2</v>
+      </c>
+      <c r="R3" s="3">
+        <v>9.0069770812988198E-2</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0.100016593933105</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0.120012760162353</v>
+      </c>
+      <c r="U3" s="3">
+        <v>9.9980831146240207E-2</v>
+      </c>
+      <c r="V3" s="3">
+        <v>8.0103874206542899E-2</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0.130064487457275</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0.110096931457519</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0.130047798156738</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0.19989013671875</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0.179989337921142</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>0.149781703948974</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0.16999006271362299</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>0.22007703781127899</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>0.179939270019531</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>0.32998085021972601</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>0.29019832611083901</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>0.32992124557495101</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>0.391693115234375</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>0.31545400619506803</v>
+      </c>
+      <c r="AK3" s="3">
+        <v>0.33997297286987299</v>
+      </c>
+      <c r="AL3" s="3">
+        <v>0.33556222915649397</v>
+      </c>
+      <c r="AM3" s="3">
+        <v>0.449769496917724</v>
+      </c>
+      <c r="AN3" s="3">
+        <v>0.38988590240478499</v>
+      </c>
+      <c r="AO3" s="3">
+        <v>0.35002231597900302</v>
+      </c>
+      <c r="AP3" s="3">
+        <v>0.36999225616455</v>
+      </c>
+      <c r="AQ3" s="3">
+        <v>0.390124320983886</v>
+      </c>
+      <c r="AR3" s="3">
+        <v>0.61012029647827104</v>
+      </c>
+      <c r="AS3" s="3">
+        <v>0.46022653579711897</v>
+      </c>
+      <c r="AT3" s="3">
+        <v>0.51031827926635698</v>
+      </c>
+      <c r="AU3" s="3">
+        <v>0.56025743484497004</v>
+      </c>
+      <c r="AV3" s="3">
+        <v>0.54018735885620095</v>
+      </c>
+      <c r="AW3" s="3">
+        <v>0.60005664825439398</v>
+      </c>
+      <c r="AX3" s="3">
+        <v>0.65973043441772405</v>
+      </c>
+      <c r="AY3" s="3">
+        <v>0.54026842117309504</v>
+      </c>
+      <c r="AZ3" s="3">
+        <v>0.65007209777831998</v>
+      </c>
+      <c r="BA3" s="3">
+        <v>0.605349540710449</v>
+      </c>
+      <c r="BB3" s="3">
+        <v>0.73635101318359297</v>
+      </c>
+      <c r="BC3" s="3">
+        <v>0.79070568084716797</v>
+      </c>
+      <c r="BD3" s="3">
+        <v>0.70060491561889604</v>
+      </c>
+      <c r="BE3" s="3">
+        <v>0.73017120361328103</v>
+      </c>
+      <c r="BF3" s="3">
+        <v>0.84960699081420898</v>
+      </c>
+      <c r="BG3" s="3">
+        <v>0.86108207702636697</v>
+      </c>
+      <c r="BH3" s="3">
+        <v>0.87027549743652299</v>
+      </c>
+      <c r="BI3" s="3">
+        <v>0.83450555801391602</v>
+      </c>
+      <c r="BJ3" s="3">
+        <v>0.83033800125122004</v>
+      </c>
+      <c r="BK3" s="3">
+        <v>1.0266923904418901</v>
+      </c>
+      <c r="BL3" s="3">
+        <v>1.0369563102722099</v>
+      </c>
+      <c r="BM3" s="3">
+        <v>0.99203348159789995</v>
+      </c>
+      <c r="BN3" s="3">
+        <v>1.1707329750061</v>
+      </c>
+      <c r="BO3" s="3">
+        <v>1.2395691871643</v>
+      </c>
+      <c r="BP3" s="3">
+        <v>0.99014520645141602</v>
+      </c>
+      <c r="BQ3" s="3">
+        <v>1.0364031791687001</v>
+      </c>
+      <c r="BR3" s="3">
+        <v>1.1202573776245099</v>
+      </c>
+      <c r="BS3" s="3">
+        <v>1.09001636505126</v>
+      </c>
+      <c r="BT3" s="3">
+        <v>1.2404704093933101</v>
+      </c>
+      <c r="BU3" s="3">
+        <v>1.24667644500732</v>
+      </c>
+      <c r="BV3" s="3">
+        <v>1.18959665298461</v>
+      </c>
+      <c r="BW3" s="3">
+        <v>1.33032798767089</v>
+      </c>
+      <c r="BX3" s="3">
+        <v>1.29984378814697</v>
+      </c>
+      <c r="BY3" s="3">
+        <v>1.27090692520141</v>
+      </c>
+      <c r="BZ3" s="3">
+        <v>1.2503457069396899</v>
+      </c>
+      <c r="CA3" s="3">
+        <v>1.6486072540283201</v>
+      </c>
+      <c r="CB3" s="3">
+        <v>1.4097142219543399</v>
+      </c>
+      <c r="CC3" s="3">
+        <v>1.69910907745361</v>
+      </c>
+      <c r="CD3" s="3">
+        <v>1.92645788192749</v>
+      </c>
+      <c r="CE3" s="3">
+        <v>1.5087532997131301</v>
+      </c>
+      <c r="CF3" s="3">
+        <v>1.9285798072814899</v>
+      </c>
+      <c r="CG3" s="3">
+        <v>1.7808985710144001</v>
+      </c>
+      <c r="CH3" s="3">
+        <v>1.69109582901</v>
+      </c>
+      <c r="CI3" s="3">
+        <v>1.77001953125</v>
+      </c>
+      <c r="CJ3" s="3">
+        <v>1.6398191452026301</v>
+      </c>
+      <c r="CK3" s="3">
+        <v>1.9621825218200599</v>
+      </c>
+      <c r="CL3" s="3">
+        <v>1.8502068519592201</v>
+      </c>
+      <c r="CM3" s="3">
+        <v>2.07061767578125</v>
+      </c>
+      <c r="CN3" s="3">
+        <v>1.80994272232055</v>
+      </c>
+      <c r="CO3" s="3">
+        <v>1.8397521972656199</v>
+      </c>
+      <c r="CP3" s="3">
+        <v>2.4657964706420898</v>
+      </c>
+      <c r="CQ3" s="3">
+        <v>2.1114373207092201</v>
+      </c>
+      <c r="CR3" s="3">
+        <v>2.1304249763488698</v>
+      </c>
+      <c r="CS3" s="3">
+        <v>2.3811006546020499</v>
+      </c>
+      <c r="CT3" s="3">
+        <v>2.5472283363342201</v>
+      </c>
+      <c r="CU3" s="3">
+        <v>2.2812438011169398</v>
+      </c>
+      <c r="CV3" s="3">
+        <v>2.0804238319396902</v>
+      </c>
+      <c r="CW3" s="3">
+        <v>2.2812294960021902</v>
+      </c>
+      <c r="CX3" s="4">
+        <v>2.2001814842224099</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>